<commit_message>
Declare COVID Winter 2020 Champion
</commit_message>
<xml_diff>
--- a/Doug - Fall 2025.xlsx
+++ b/Doug - Fall 2025.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sbclaude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5DBECFD-B95D-412F-9173-42475B4C8E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58D6C3F-F6AE-4054-B664-C598F67DC826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_Teams" sheetId="1" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="419">
   <si>
     <t>Team_Name</t>
   </si>
@@ -1158,13 +1159,145 @@
   </si>
   <si>
     <t>Xtreme</t>
+  </si>
+  <si>
+    <t>Division One - Fall 2025 Schedule</t>
+  </si>
+  <si>
+    <t>All games played at the Saddlebrook Complex</t>
+  </si>
+  <si>
+    <t>9:00</t>
+  </si>
+  <si>
+    <t>10:30</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Away</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>09-05</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>09-10</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>09-12</t>
+  </si>
+  <si>
+    <t>09-17</t>
+  </si>
+  <si>
+    <t>09-19</t>
+  </si>
+  <si>
+    <t>09-24</t>
+  </si>
+  <si>
+    <t>09-26</t>
+  </si>
+  <si>
+    <t>10-01</t>
+  </si>
+  <si>
+    <t>10-03</t>
+  </si>
+  <si>
+    <t>10-08</t>
+  </si>
+  <si>
+    <t>10-10</t>
+  </si>
+  <si>
+    <t>10-15</t>
+  </si>
+  <si>
+    <t>10-17</t>
+  </si>
+  <si>
+    <t>NO GAMES - FIELDS CLOSED FOR VILLAGES TOURNAMENT</t>
+  </si>
+  <si>
+    <t>10-22</t>
+  </si>
+  <si>
+    <t>10-24</t>
+  </si>
+  <si>
+    <t>10-29</t>
+  </si>
+  <si>
+    <t>10-31</t>
+  </si>
+  <si>
+    <t>11-05</t>
+  </si>
+  <si>
+    <t>11-07</t>
+  </si>
+  <si>
+    <t>11-12</t>
+  </si>
+  <si>
+    <t>11-14</t>
+  </si>
+  <si>
+    <t>11-19</t>
+  </si>
+  <si>
+    <t>11-21</t>
+  </si>
+  <si>
+    <t>11-26</t>
+  </si>
+  <si>
+    <t>RAIN-OUT MAKEUP OR POST SEASON PLAYOFFS</t>
+  </si>
+  <si>
+    <t>11-28</t>
+  </si>
+  <si>
+    <t>TURKEY BOWL - THANKSGIVING TOURNAMENT</t>
+  </si>
+  <si>
+    <t>12-3</t>
+  </si>
+  <si>
+    <t>POST SEASON PLAYOFFS</t>
+  </si>
+  <si>
+    <t>12-5</t>
+  </si>
+  <si>
+    <t>12-10</t>
+  </si>
+  <si>
+    <t>POST SEASON PLAYOFFS - IF NECESSARY</t>
+  </si>
+  <si>
+    <t>12-12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1178,13 +1311,48 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1214,7 +1382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1222,6 +1390,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -4443,4 +4638,1740 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8D2E25-286A-4490-A61A-9FFE818B6EDF}">
+  <dimension ref="A1:T33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="7" style="2" customWidth="1"/>
+    <col min="10" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="5" style="2" customWidth="1"/>
+    <col min="16" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E4" t="s">
+        <v>382</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" t="s">
+        <v>381</v>
+      </c>
+      <c r="H4" t="s">
+        <v>382</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J4" t="s">
+        <v>381</v>
+      </c>
+      <c r="K4" t="s">
+        <v>382</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="M4" t="s">
+        <v>381</v>
+      </c>
+      <c r="N4" t="s">
+        <v>382</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="P4" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>382</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="S4" t="s">
+        <v>381</v>
+      </c>
+      <c r="T4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>374</v>
+      </c>
+      <c r="E5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K5" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O5" s="2">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>345</v>
+      </c>
+      <c r="R5" s="2">
+        <v>4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>230</v>
+      </c>
+      <c r="T5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B6" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>345</v>
+      </c>
+      <c r="K6" t="s">
+        <v>314</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>286</v>
+      </c>
+      <c r="N6" t="s">
+        <v>139</v>
+      </c>
+      <c r="O6" s="2">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>230</v>
+      </c>
+      <c r="R6" s="2">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>259</v>
+      </c>
+      <c r="T6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>374</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>201</v>
+      </c>
+      <c r="K7" t="s">
+        <v>286</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>259</v>
+      </c>
+      <c r="N7" t="s">
+        <v>314</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>108</v>
+      </c>
+      <c r="R7" s="2">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>230</v>
+      </c>
+      <c r="T7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>286</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>314</v>
+      </c>
+      <c r="H8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>259</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>374</v>
+      </c>
+      <c r="N8" t="s">
+        <v>230</v>
+      </c>
+      <c r="O8" s="2">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>345</v>
+      </c>
+      <c r="R8" s="2">
+        <v>4</v>
+      </c>
+      <c r="S8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>389</v>
+      </c>
+      <c r="B9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" t="s">
+        <v>374</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" t="s">
+        <v>345</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>286</v>
+      </c>
+      <c r="N9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>201</v>
+      </c>
+      <c r="R9" s="2">
+        <v>4</v>
+      </c>
+      <c r="S9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>314</v>
+      </c>
+      <c r="H10" t="s">
+        <v>201</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K10" t="s">
+        <v>139</v>
+      </c>
+      <c r="L10" s="2">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>171</v>
+      </c>
+      <c r="N10" t="s">
+        <v>259</v>
+      </c>
+      <c r="O10" s="2">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="2">
+        <v>4</v>
+      </c>
+      <c r="S10" t="s">
+        <v>374</v>
+      </c>
+      <c r="T10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>391</v>
+      </c>
+      <c r="B11" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>230</v>
+      </c>
+      <c r="H11" t="s">
+        <v>314</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>286</v>
+      </c>
+      <c r="K11" t="s">
+        <v>259</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>171</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="2">
+        <v>3</v>
+      </c>
+      <c r="P11" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>374</v>
+      </c>
+      <c r="R11" s="2">
+        <v>4</v>
+      </c>
+      <c r="S11" t="s">
+        <v>201</v>
+      </c>
+      <c r="T11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>392</v>
+      </c>
+      <c r="B12" t="s">
+        <v>386</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>230</v>
+      </c>
+      <c r="H12" t="s">
+        <v>171</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>259</v>
+      </c>
+      <c r="K12" t="s">
+        <v>345</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>108</v>
+      </c>
+      <c r="N12" t="s">
+        <v>314</v>
+      </c>
+      <c r="O12" s="2">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>286</v>
+      </c>
+      <c r="R12" s="2">
+        <v>4</v>
+      </c>
+      <c r="S12" t="s">
+        <v>374</v>
+      </c>
+      <c r="T12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>393</v>
+      </c>
+      <c r="B13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>374</v>
+      </c>
+      <c r="E13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+      <c r="J13" t="s">
+        <v>286</v>
+      </c>
+      <c r="K13" t="s">
+        <v>230</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>345</v>
+      </c>
+      <c r="N13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="2">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R13" s="2">
+        <v>4</v>
+      </c>
+      <c r="S13" t="s">
+        <v>314</v>
+      </c>
+      <c r="T13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>374</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>286</v>
+      </c>
+      <c r="H14" t="s">
+        <v>171</v>
+      </c>
+      <c r="I14" s="2">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>139</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="2">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>345</v>
+      </c>
+      <c r="N14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3</v>
+      </c>
+      <c r="P14" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>201</v>
+      </c>
+      <c r="R14" s="2">
+        <v>4</v>
+      </c>
+      <c r="S14" t="s">
+        <v>41</v>
+      </c>
+      <c r="T14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B15" t="s">
+        <v>384</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>286</v>
+      </c>
+      <c r="E15" t="s">
+        <v>314</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>345</v>
+      </c>
+      <c r="H15" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>374</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="2">
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>139</v>
+      </c>
+      <c r="N15" t="s">
+        <v>230</v>
+      </c>
+      <c r="O15" s="2">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>108</v>
+      </c>
+      <c r="R15" s="2">
+        <v>4</v>
+      </c>
+      <c r="S15" t="s">
+        <v>76</v>
+      </c>
+      <c r="T15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16" t="s">
+        <v>386</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>345</v>
+      </c>
+      <c r="E16" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>201</v>
+      </c>
+      <c r="H16" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="2">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" t="s">
+        <v>259</v>
+      </c>
+      <c r="O16" s="2">
+        <v>3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>374</v>
+      </c>
+      <c r="R16" s="2">
+        <v>4</v>
+      </c>
+      <c r="S16" t="s">
+        <v>171</v>
+      </c>
+      <c r="T16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>397</v>
+      </c>
+      <c r="B17" t="s">
+        <v>384</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="13"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>399</v>
+      </c>
+      <c r="B18" t="s">
+        <v>386</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>374</v>
+      </c>
+      <c r="E18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>230</v>
+      </c>
+      <c r="K18" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="2">
+        <v>2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>171</v>
+      </c>
+      <c r="N18" t="s">
+        <v>201</v>
+      </c>
+      <c r="O18" s="2">
+        <v>3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>286</v>
+      </c>
+      <c r="R18" s="2">
+        <v>4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>314</v>
+      </c>
+      <c r="T18" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>400</v>
+      </c>
+      <c r="B19" t="s">
+        <v>384</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>314</v>
+      </c>
+      <c r="H19" t="s">
+        <v>259</v>
+      </c>
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>345</v>
+      </c>
+      <c r="K19" t="s">
+        <v>139</v>
+      </c>
+      <c r="L19" s="2">
+        <v>2</v>
+      </c>
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" t="s">
+        <v>230</v>
+      </c>
+      <c r="O19" s="2">
+        <v>3</v>
+      </c>
+      <c r="P19" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>76</v>
+      </c>
+      <c r="R19" s="2">
+        <v>4</v>
+      </c>
+      <c r="S19" t="s">
+        <v>286</v>
+      </c>
+      <c r="T19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>401</v>
+      </c>
+      <c r="B20" t="s">
+        <v>386</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" t="s">
+        <v>314</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>345</v>
+      </c>
+      <c r="H20" t="s">
+        <v>201</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>230</v>
+      </c>
+      <c r="K20" t="s">
+        <v>374</v>
+      </c>
+      <c r="L20" s="2">
+        <v>2</v>
+      </c>
+      <c r="M20" t="s">
+        <v>259</v>
+      </c>
+      <c r="N20" t="s">
+        <v>76</v>
+      </c>
+      <c r="O20" s="2">
+        <v>3</v>
+      </c>
+      <c r="P20" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>108</v>
+      </c>
+      <c r="R20" s="2">
+        <v>4</v>
+      </c>
+      <c r="S20" t="s">
+        <v>171</v>
+      </c>
+      <c r="T20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>402</v>
+      </c>
+      <c r="B21" t="s">
+        <v>384</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>286</v>
+      </c>
+      <c r="I21" s="2">
+        <v>4</v>
+      </c>
+      <c r="J21" t="s">
+        <v>314</v>
+      </c>
+      <c r="K21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="2">
+        <v>2</v>
+      </c>
+      <c r="M21" t="s">
+        <v>345</v>
+      </c>
+      <c r="N21" t="s">
+        <v>108</v>
+      </c>
+      <c r="O21" s="2">
+        <v>3</v>
+      </c>
+      <c r="P21" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>230</v>
+      </c>
+      <c r="R21" s="2">
+        <v>4</v>
+      </c>
+      <c r="S21" t="s">
+        <v>374</v>
+      </c>
+      <c r="T21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>403</v>
+      </c>
+      <c r="B22" t="s">
+        <v>386</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>345</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>286</v>
+      </c>
+      <c r="H22" t="s">
+        <v>374</v>
+      </c>
+      <c r="I22" s="2">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>259</v>
+      </c>
+      <c r="K22" t="s">
+        <v>171</v>
+      </c>
+      <c r="L22" s="2">
+        <v>2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>201</v>
+      </c>
+      <c r="N22" t="s">
+        <v>314</v>
+      </c>
+      <c r="O22" s="2">
+        <v>3</v>
+      </c>
+      <c r="P22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>230</v>
+      </c>
+      <c r="R22" s="2">
+        <v>4</v>
+      </c>
+      <c r="S22" t="s">
+        <v>139</v>
+      </c>
+      <c r="T22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>404</v>
+      </c>
+      <c r="B23" t="s">
+        <v>384</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="2">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I23" s="2">
+        <v>4</v>
+      </c>
+      <c r="J23" t="s">
+        <v>314</v>
+      </c>
+      <c r="K23" t="s">
+        <v>230</v>
+      </c>
+      <c r="L23" s="2">
+        <v>2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>374</v>
+      </c>
+      <c r="N23" t="s">
+        <v>345</v>
+      </c>
+      <c r="O23" s="2">
+        <v>3</v>
+      </c>
+      <c r="P23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>41</v>
+      </c>
+      <c r="R23" s="2">
+        <v>4</v>
+      </c>
+      <c r="S23" t="s">
+        <v>259</v>
+      </c>
+      <c r="T23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>405</v>
+      </c>
+      <c r="B24" t="s">
+        <v>386</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>286</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" t="s">
+        <v>230</v>
+      </c>
+      <c r="I24" s="2">
+        <v>4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>345</v>
+      </c>
+      <c r="K24" t="s">
+        <v>259</v>
+      </c>
+      <c r="L24" s="2">
+        <v>2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>139</v>
+      </c>
+      <c r="N24" t="s">
+        <v>374</v>
+      </c>
+      <c r="O24" s="2">
+        <v>3</v>
+      </c>
+      <c r="P24" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>108</v>
+      </c>
+      <c r="R24" s="2">
+        <v>4</v>
+      </c>
+      <c r="S24" t="s">
+        <v>201</v>
+      </c>
+      <c r="T24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>406</v>
+      </c>
+      <c r="B25" t="s">
+        <v>384</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25" t="s">
+        <v>259</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>201</v>
+      </c>
+      <c r="K25" t="s">
+        <v>374</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>171</v>
+      </c>
+      <c r="N25" t="s">
+        <v>314</v>
+      </c>
+      <c r="O25" s="2">
+        <v>3</v>
+      </c>
+      <c r="P25" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>345</v>
+      </c>
+      <c r="R25" s="2">
+        <v>4</v>
+      </c>
+      <c r="S25" t="s">
+        <v>230</v>
+      </c>
+      <c r="T25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>407</v>
+      </c>
+      <c r="B26" t="s">
+        <v>386</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" t="s">
+        <v>286</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>314</v>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>108</v>
+      </c>
+      <c r="K26" t="s">
+        <v>374</v>
+      </c>
+      <c r="L26" s="2">
+        <v>2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>230</v>
+      </c>
+      <c r="N26" t="s">
+        <v>345</v>
+      </c>
+      <c r="O26" s="2">
+        <v>3</v>
+      </c>
+      <c r="P26" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>259</v>
+      </c>
+      <c r="R26" s="2">
+        <v>4</v>
+      </c>
+      <c r="S26" t="s">
+        <v>76</v>
+      </c>
+      <c r="T26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>408</v>
+      </c>
+      <c r="B27" t="s">
+        <v>384</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>259</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>171</v>
+      </c>
+      <c r="H27" t="s">
+        <v>345</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>230</v>
+      </c>
+      <c r="K27" t="s">
+        <v>139</v>
+      </c>
+      <c r="L27" s="2">
+        <v>2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>314</v>
+      </c>
+      <c r="N27" t="s">
+        <v>286</v>
+      </c>
+      <c r="O27" s="2">
+        <v>3</v>
+      </c>
+      <c r="P27" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>374</v>
+      </c>
+      <c r="R27" s="2">
+        <v>4</v>
+      </c>
+      <c r="S27" t="s">
+        <v>201</v>
+      </c>
+      <c r="T27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="B28" t="s">
+        <v>384</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="13"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="B29" t="s">
+        <v>384</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="13"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B30" t="s">
+        <v>384</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="13"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="B31" t="s">
+        <v>384</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="13"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="B32" t="s">
+        <v>384</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="13"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="B33" t="s">
+        <v>384</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C29:S29"/>
+    <mergeCell ref="C30:S30"/>
+    <mergeCell ref="C31:S31"/>
+    <mergeCell ref="C32:S32"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L3:T3"/>
+    <mergeCell ref="C17:S17"/>
+    <mergeCell ref="C28:S28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>